<commit_message>
Final Submit after 1st Test
</commit_message>
<xml_diff>
--- a/ans.xlsx
+++ b/ans.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Advanced-QNA-RAG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1E03ED-FA21-4C65-ADA1-0A6E13D97992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2FB72C-7088-44DA-B0B5-86836A1C435E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1080" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>In the context of the excerpt, how does the narrator’s invocation of the Sanskrit shloka and her father’s words illustrate the interplay between personal legacy and societal impact in her efforts to end the devadasi system?</t>
   </si>
@@ -43,13 +44,94 @@
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <t>How did the narrator’s academic success influence her social standing and relationships with her male classmates over time?</t>
+  </si>
+  <si>
+    <t>Her academic achievements earned her respect and popularity as both a doctor and teacher, raising her social standing in a community that rarely saw women excel academically. However, because the conservative culture discouraged boys and girls from interacting, her success also made many male classmates uneasy, creating a distance that persisted despite her growing reputation.</t>
+  </si>
+  <si>
+    <t>Her resilience let her reframe the gender‑bias narrative—questioning the status quo, persisting despite loneliness and health strain, and turning the fear of being the sole woman into a source of determination—while her focus on education provided a concrete goal, the support of mentors who celebrated her breakthrough, and the skills that transformed her from a scared teenager into a confident, capable engineer, enabling her to cope with the emotional challenges of isolation. In short, by reshaping her mindset, drawing encouragement from others, and letting her studies anchor her identity, she turned adversity into confidence and perseverance.</t>
+  </si>
+  <si>
+    <t>In what ways did the narrator’s resilience and focus on education help her cope with the emotional challenges of being the only woman in her engineering class?</t>
+  </si>
+  <si>
+    <t>Why did the narrator find the lunch at Rekha’s house different from what she expected, and how did she react to it?</t>
+  </si>
+  <si>
+    <t>The narrator realized the lunch was different because it had been prepared for a shraddha ceremony—so the dishes were intentionally simple, bland, and “hospital‑food”‑like rather than the flavorful fare she expected. She responded with good‑natured humor, quipping, “I may wear a simple sari but I am a foodie, Rekha! Is the lunch specially arranged so that I don’t come again?” and later playfully reached for a banana and hoped for dessert.</t>
+  </si>
+  <si>
+    <t>What does the conversation about “indigenous vegetables” reveal about the narrator’s understanding of traditional customs and food culture?</t>
+  </si>
+  <si>
+    <t>The dialogue shows that the narrator initially assumes all vegetables used in Indian meals are truly native, revealing a superficial grasp of traditional customs and food culture. His uncle’s explanation that staples like tomatoes, chillies, corn, groundnut and beans were introduced from abroad (via Portuguese, British, etc.) forces the narrator to recognize that many “indigenous” foods are actually foreign imports that have become woven into Indian culinary tradition.</t>
+  </si>
+  <si>
+    <t>According to Avva, how does Bhairavnath manage to help multiple people return from Kashi simultaneously, and what special ability does he possess that enables this?</t>
+  </si>
+  <si>
+    <t>Why do people in south India keep Gangajal (holy water from the Ganga) in their homes, and what is its primary purpose according to Avva's explanation?</t>
+  </si>
+  <si>
+    <t>At Indira Ajji's house, what was the significance of the single banana leaf laid out with various dishes and desserts, and who was this food intended for?</t>
+  </si>
+  <si>
+    <t>According to Avva, Bhairavnath assists each devotee by accompanying them in his **invisible form** until they safely reach home, then instantly returns to help the next pilgrim. His special ability is this invisibility, which lets him travel unseen and quickly move between devotees.</t>
+  </si>
+  <si>
+    <t>People in south India keep a few spoons of Gangajal in their homes because they believe the holy water can aid a person who is in the last days of life. According to Avva, its primary purpose is to help that dying individual attain heaven.</t>
+  </si>
+  <si>
+    <t>The single banana leaf, set among the flowers and laden with dishes and desserts, serves as a traditional, festive presentation of food at Indira Ajji’s house, but the passage does not explain any specific symbolic meaning. Likewise, the text does not state who the food was intended for.</t>
+  </si>
+  <si>
+    <t>Where was the author waiting and what type of Indian clothes was she wearing?</t>
+  </si>
+  <si>
+    <t>What did the well-dressed woman tell the author about the business class line, and what insulting name did she use?</t>
+  </si>
+  <si>
+    <t>According to the woman, what are two special benefits that business class passengers get compared to economy class?</t>
+  </si>
+  <si>
+    <t>The author was waiting at the Indian wedding ceremony where she had been asked to deliver flowers, and she was dressed in a two‑hundred‑rupee sari with a big bindi, a mangalsutra and glass bangles, presenting herself as the stereotypical “bharatiya nari.”</t>
+  </si>
+  <si>
+    <t>She told the author that the line he was in was intended only for business‑class travelers and pointed him toward the economy‑class queue. The insulting term she used for the economy line was “cattle class.”</t>
+  </si>
+  <si>
+    <t>The woman explains that business‑class passengers enjoy two special perks over economy travelers: **they are given priority on arrival (they “come first”)** and **they earn more frequent‑flyer miles for the same flight**. This reasoning comes directly from her statement that “they will come first upon arrival and we get more frequent flyer miles for the same flight,” which she cites as the advantages of holding a business‑class ticket.</t>
+  </si>
+  <si>
+    <t>Why did Binya start closing her umbrella when passing Ram Bharosa’s shop?</t>
+  </si>
+  <si>
+    <t>Binya began closing her umbrella as she passed Ram Bharosa’s shop because she had decided she no longer needed it after giving it to him in exchange for a toffee. Closing it signaled that she was returning the umbrella to its folded state, reflecting her change of mind about keeping it.</t>
+  </si>
+  <si>
+    <t>What does Binya’s internal conflict about the umbrella reveal about her character?</t>
+  </si>
+  <si>
+    <t>Binya’s internal conflict-refusing to sell the umbrella even for a higher price and later chasing it as the wind tosses it away-shows that she places sentimental and principled value on the object rather than material gain, revealing her as emotionally driven and guided by personal integrity. Her remark that “an umbrella isn’t everything” underscores that she prioritizes deeper values and relationships over simple financial benefit.</t>
+  </si>
+  <si>
+    <t>What is the symbolic significance of Ram Bharosa returning the umbrella to Binya, and how does it transform their relationship?</t>
+  </si>
+  <si>
+    <t>In the story, when Ram Bharosa finally gives the blue umbrella back to Binya, the act becomes a concrete symbol of his repentance and the surrender of the envy that had driven him to steal it. By returning the umbrella he not only restores Binya’s trust but also demonstrates humility and forgiveness, turning their relationship from one marked by greed and rivalry into a bond of mutual respect, compassion and genuine friendship.</t>
+  </si>
+  <si>
+    <t>uvicorn app:app --host 0.0.0.0 --port 8080 --reload</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,16 +139,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -74,12 +169,152 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -95,6 +330,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>545468</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>87101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0493AF28-8B3D-2253-A4E6-F0F8A41E4DAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="542925"/>
+          <a:ext cx="18223868" cy="9859751"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>412100</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>144284</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E063E42-19D5-FA7F-BC0E-BD4B34683777}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="10858500"/>
+          <a:ext cx="18090500" cy="10097909"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>583574</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>106204</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F58C044C-2536-0631-4150-F58EFB6C8181}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="21536025"/>
+          <a:ext cx="18261974" cy="10240804"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -360,42 +732,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C4"/>
+  <dimension ref="B2:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="196.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="100" style="1" customWidth="1"/>
+    <col min="3" max="3" width="119.77734375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="2" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="3" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="4" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D468F771-4B80-4359-BE9A-5126046CA549}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>